<commit_message>
Iteración 4 a medias
</commit_message>
<xml_diff>
--- a/DiarioProyecto.xlsx
+++ b/DiarioProyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javie\OneDrive\Escritorio\Proyecto-TT1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9FFC9C-2D86-469F-B41C-4042E219FD5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AF8F8B-10A1-4DF4-AB75-8E4ED191CEEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{171297B1-7AE2-B240-830B-C3611B6C68F6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="96">
   <si>
     <t>Accel.m</t>
   </si>
@@ -380,6 +380,27 @@
     <t>Difícil. Pasar funciones como parámetros y utilizar clases de
 integración numérica externas. Hay que hacer un bypass a código.
 No he tenido tiempo esta iteración.</t>
+  </si>
+  <si>
+    <t>Fácil (una vez te funciona EqnEquinox jeje).</t>
+  </si>
+  <si>
+    <t>Fácil, necesita gast implementada antes.</t>
+  </si>
+  <si>
+    <t>Normal. Hay que tener cuidado con las cadenas en C++ (acaban
+en '\0'.</t>
+  </si>
+  <si>
+    <t>Normal.</t>
+  </si>
+  <si>
+    <t>Se me complicó porque no obtenía los valores correctos, por
+culpa de inicializar mal un valor de AuxParam.</t>
+  </si>
+  <si>
+    <t>Como no tengo debugger, solucioné el problema imprimiendo por
+pantalla todos los resultados parciales tanto en C++ como Matlab.</t>
   </si>
 </sst>
 </file>
@@ -554,6 +575,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -562,12 +589,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -885,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EB0CE-B6BF-CB4D-BCAF-F7FB8362BFF6}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -901,26 +922,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
     </row>
     <row r="3" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -949,11 +970,21 @@
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="3"/>
+      <c r="B4" s="5">
+        <v>45428</v>
+      </c>
+      <c r="C4" s="5">
+        <v>45428</v>
+      </c>
+      <c r="D4" s="8">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E4" s="8">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
@@ -1047,25 +1078,25 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="19">
         <v>45391</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="G9" s="21"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -1075,7 +1106,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="3"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1147,11 +1178,21 @@
       <c r="A14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="3"/>
+      <c r="B14" s="5">
+        <v>45427</v>
+      </c>
+      <c r="C14" s="5">
+        <v>45427</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="E14" s="8">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1313,7 +1354,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="E22" s="8">
-        <v>0.125</v>
+        <v>0.1736111111111111</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>87</v>
@@ -1578,18 +1619,30 @@
       <c r="F34" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
+      <c r="B35" s="5">
+        <v>45428</v>
+      </c>
+      <c r="C35" s="5">
+        <v>45429</v>
+      </c>
+      <c r="D35" s="8">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E35" s="8">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
@@ -1624,11 +1677,15 @@
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
+      <c r="B38" s="5">
+        <v>45427</v>
+      </c>
+      <c r="C38" s="5">
+        <v>45427</v>
+      </c>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="3"/>
@@ -1672,22 +1729,42 @@
       <c r="A41" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="7"/>
+      <c r="B41" s="5">
+        <v>45427</v>
+      </c>
+      <c r="C41" s="5">
+        <v>45427</v>
+      </c>
+      <c r="D41" s="8">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="E41" s="8">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="3"/>
+      <c r="B42" s="5">
+        <v>45427</v>
+      </c>
+      <c r="C42" s="5">
+        <v>45427</v>
+      </c>
+      <c r="D42" s="8">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E42" s="8">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>92</v>
+      </c>
       <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -1715,11 +1792,19 @@
       <c r="A44" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="3"/>
+      <c r="B44" s="5">
+        <v>45427</v>
+      </c>
       <c r="C44" s="3"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="3"/>
+      <c r="D44" s="8">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E44" s="8">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -1793,11 +1878,11 @@
       </c>
       <c r="D48" s="8">
         <f>SUM(D4:D47)</f>
-        <v>0.93402777777777846</v>
+        <v>1.1041666666666672</v>
       </c>
       <c r="E48" s="8">
         <f>SUM(E4:E47)</f>
-        <v>1.4722222222222219</v>
+        <v>1.7569444444444442</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>77</v>
@@ -1818,5 +1903,6 @@
     <mergeCell ref="A2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>